<commit_message>
intento de cambio a listArray
</commit_message>
<xml_diff>
--- a/Data/Paises.xlsx
+++ b/Data/Paises.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e351fcecb347c58/Escritorio/U/Progra 1/Java Project/Proyecto/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e351fcecb347c58/Escritorio/U/Progra 1/Java Project/JavaProject/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{231D6E0D-48E9-43E5-83E4-07552FA489D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E4B36A2-C7B6-429A-A7D0-6D7EF7AC332F}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="8_{231D6E0D-48E9-43E5-83E4-07552FA489D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E82DA8E-B17F-4641-BF6F-695704A96B4E}"/>
   <bookViews>
-    <workbookView xWindow="-29412" yWindow="1368" windowWidth="38700" windowHeight="15432" activeTab="1" xr2:uid="{C4731804-0404-4395-AE7B-C32DE555072D}"/>
+    <workbookView xWindow="-38400" yWindow="3900" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{C4731804-0404-4395-AE7B-C32DE555072D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$E$249</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet2!$A$1:$E$249</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2556" uniqueCount="1759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2579" uniqueCount="1766">
   <si>
     <r>
       <t>ISO 3166-1</t>
@@ -10246,6 +10247,27 @@
   </si>
   <si>
     <t>INSERT INTO project.paises (`Pais`, `2Iso`, `ISO`) VALUES (</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>Estados unidos</t>
+  </si>
+  <si>
+    <t>Francia</t>
+  </si>
+  <si>
+    <t>Italia</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>listaPaises.add(</t>
+  </si>
+  <si>
+    <t>);</t>
   </si>
 </sst>
 </file>
@@ -10505,6 +10527,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -10512,6 +10543,27 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -10523,24 +10575,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -10549,18 +10583,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -28555,17 +28577,20 @@
   <dimension ref="A1:H287"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="35"/>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
@@ -28627,16 +28652,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
     </row>
     <row r="5" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -28951,16 +28976,16 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="22"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="25"/>
     </row>
     <row r="18" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
@@ -29333,22 +29358,22 @@
       <c r="B32" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="E32" s="29" t="s">
+      <c r="E32" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="F32" s="29">
+      <c r="F32" s="21">
         <v>535</v>
       </c>
-      <c r="G32" s="29" t="s">
+      <c r="G32" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="H32" s="32" t="s">
+      <c r="H32" s="36" t="s">
         <v>187</v>
       </c>
     </row>
@@ -29356,25 +29381,25 @@
       <c r="A33" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="33"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="37"/>
     </row>
     <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="34"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="38"/>
     </row>
     <row r="35" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
@@ -29507,16 +29532,16 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="22"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="25"/>
     </row>
     <row r="41" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
@@ -29597,16 +29622,16 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="23" t="s">
         <v>238</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="22"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="25"/>
     </row>
     <row r="45" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
@@ -29739,28 +29764,28 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="35" t="s">
+      <c r="A50" s="29" t="s">
         <v>269</v>
       </c>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="37"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="31"/>
     </row>
     <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="20" t="s">
+      <c r="A51" s="23" t="s">
         <v>270</v>
       </c>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="21"/>
-      <c r="H51" s="22"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="25"/>
     </row>
     <row r="52" spans="1:8" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
@@ -29893,16 +29918,16 @@
       </c>
     </row>
     <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="20" t="s">
+      <c r="A57" s="23" t="s">
         <v>301</v>
       </c>
-      <c r="B57" s="21"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
-      <c r="H57" s="22"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="24"/>
+      <c r="H57" s="25"/>
     </row>
     <row r="58" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
@@ -29931,16 +29956,16 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="20" t="s">
+      <c r="A59" s="23" t="s">
         <v>309</v>
       </c>
-      <c r="B59" s="21"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
-      <c r="E59" s="21"/>
-      <c r="F59" s="21"/>
-      <c r="G59" s="21"/>
-      <c r="H59" s="22"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="25"/>
     </row>
     <row r="60" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
@@ -30099,16 +30124,16 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="20" t="s">
+      <c r="A66" s="23" t="s">
         <v>347</v>
       </c>
-      <c r="B66" s="21"/>
-      <c r="C66" s="21"/>
-      <c r="D66" s="21"/>
-      <c r="E66" s="21"/>
-      <c r="F66" s="21"/>
-      <c r="G66" s="21"/>
-      <c r="H66" s="22"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="24"/>
+      <c r="D66" s="24"/>
+      <c r="E66" s="24"/>
+      <c r="F66" s="24"/>
+      <c r="G66" s="24"/>
+      <c r="H66" s="25"/>
     </row>
     <row r="67" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
@@ -30293,28 +30318,28 @@
       </c>
     </row>
     <row r="74" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="35" t="s">
+      <c r="A74" s="29" t="s">
         <v>390</v>
       </c>
-      <c r="B74" s="36"/>
-      <c r="C74" s="36"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="36"/>
-      <c r="F74" s="36"/>
-      <c r="G74" s="36"/>
-      <c r="H74" s="37"/>
+      <c r="B74" s="30"/>
+      <c r="C74" s="30"/>
+      <c r="D74" s="30"/>
+      <c r="E74" s="30"/>
+      <c r="F74" s="30"/>
+      <c r="G74" s="30"/>
+      <c r="H74" s="31"/>
     </row>
     <row r="75" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="35" t="s">
+      <c r="A75" s="29" t="s">
         <v>391</v>
       </c>
-      <c r="B75" s="36"/>
-      <c r="C75" s="36"/>
-      <c r="D75" s="36"/>
-      <c r="E75" s="36"/>
-      <c r="F75" s="36"/>
-      <c r="G75" s="36"/>
-      <c r="H75" s="37"/>
+      <c r="B75" s="30"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="30"/>
+      <c r="F75" s="30"/>
+      <c r="G75" s="30"/>
+      <c r="H75" s="31"/>
     </row>
     <row r="76" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
@@ -30421,16 +30446,16 @@
       </c>
     </row>
     <row r="80" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="35" t="s">
+      <c r="A80" s="29" t="s">
         <v>416</v>
       </c>
-      <c r="B80" s="36"/>
-      <c r="C80" s="36"/>
-      <c r="D80" s="36"/>
-      <c r="E80" s="36"/>
-      <c r="F80" s="36"/>
-      <c r="G80" s="36"/>
-      <c r="H80" s="37"/>
+      <c r="B80" s="30"/>
+      <c r="C80" s="30"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="30"/>
+      <c r="F80" s="30"/>
+      <c r="G80" s="30"/>
+      <c r="H80" s="31"/>
     </row>
     <row r="81" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
@@ -30511,16 +30536,16 @@
       </c>
     </row>
     <row r="84" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="20" t="s">
+      <c r="A84" s="23" t="s">
         <v>435</v>
       </c>
-      <c r="B84" s="21"/>
-      <c r="C84" s="21"/>
-      <c r="D84" s="21"/>
-      <c r="E84" s="21"/>
-      <c r="F84" s="21"/>
-      <c r="G84" s="21"/>
-      <c r="H84" s="22"/>
+      <c r="B84" s="24"/>
+      <c r="C84" s="24"/>
+      <c r="D84" s="24"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="24"/>
+      <c r="H84" s="25"/>
     </row>
     <row r="85" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
@@ -31017,16 +31042,16 @@
       </c>
     </row>
     <row r="104" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="35" t="s">
+      <c r="A104" s="29" t="s">
         <v>552</v>
       </c>
-      <c r="B104" s="36"/>
-      <c r="C104" s="36"/>
-      <c r="D104" s="36"/>
-      <c r="E104" s="36"/>
-      <c r="F104" s="36"/>
-      <c r="G104" s="36"/>
-      <c r="H104" s="37"/>
+      <c r="B104" s="30"/>
+      <c r="C104" s="30"/>
+      <c r="D104" s="30"/>
+      <c r="E104" s="30"/>
+      <c r="F104" s="30"/>
+      <c r="G104" s="30"/>
+      <c r="H104" s="31"/>
     </row>
     <row r="105" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
@@ -31315,16 +31340,16 @@
       </c>
     </row>
     <row r="116" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="20" t="s">
+      <c r="A116" s="23" t="s">
         <v>620</v>
       </c>
-      <c r="B116" s="21"/>
-      <c r="C116" s="21"/>
-      <c r="D116" s="21"/>
-      <c r="E116" s="21"/>
-      <c r="F116" s="21"/>
-      <c r="G116" s="21"/>
-      <c r="H116" s="22"/>
+      <c r="B116" s="24"/>
+      <c r="C116" s="24"/>
+      <c r="D116" s="24"/>
+      <c r="E116" s="24"/>
+      <c r="F116" s="24"/>
+      <c r="G116" s="24"/>
+      <c r="H116" s="25"/>
     </row>
     <row r="117" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="8" t="s">
@@ -31691,16 +31716,16 @@
       </c>
     </row>
     <row r="131" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="35" t="s">
+      <c r="A131" s="29" t="s">
         <v>707</v>
       </c>
-      <c r="B131" s="36"/>
-      <c r="C131" s="36"/>
-      <c r="D131" s="36"/>
-      <c r="E131" s="36"/>
-      <c r="F131" s="36"/>
-      <c r="G131" s="36"/>
-      <c r="H131" s="37"/>
+      <c r="B131" s="30"/>
+      <c r="C131" s="30"/>
+      <c r="D131" s="30"/>
+      <c r="E131" s="30"/>
+      <c r="F131" s="30"/>
+      <c r="G131" s="30"/>
+      <c r="H131" s="31"/>
     </row>
     <row r="132" spans="1:8" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
@@ -31729,16 +31754,16 @@
       </c>
     </row>
     <row r="133" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="20" t="s">
+      <c r="A133" s="23" t="s">
         <v>714</v>
       </c>
-      <c r="B133" s="21"/>
-      <c r="C133" s="21"/>
-      <c r="D133" s="21"/>
-      <c r="E133" s="21"/>
-      <c r="F133" s="21"/>
-      <c r="G133" s="21"/>
-      <c r="H133" s="22"/>
+      <c r="B133" s="24"/>
+      <c r="C133" s="24"/>
+      <c r="D133" s="24"/>
+      <c r="E133" s="24"/>
+      <c r="F133" s="24"/>
+      <c r="G133" s="24"/>
+      <c r="H133" s="25"/>
     </row>
     <row r="134" spans="1:8" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
@@ -33119,28 +33144,28 @@
       </c>
     </row>
     <row r="187" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="35" t="s">
+      <c r="A187" s="29" t="s">
         <v>1032</v>
       </c>
-      <c r="B187" s="36"/>
-      <c r="C187" s="36"/>
-      <c r="D187" s="36"/>
-      <c r="E187" s="36"/>
-      <c r="F187" s="36"/>
-      <c r="G187" s="36"/>
-      <c r="H187" s="37"/>
+      <c r="B187" s="30"/>
+      <c r="C187" s="30"/>
+      <c r="D187" s="30"/>
+      <c r="E187" s="30"/>
+      <c r="F187" s="30"/>
+      <c r="G187" s="30"/>
+      <c r="H187" s="31"/>
     </row>
     <row r="188" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="20" t="s">
+      <c r="A188" s="23" t="s">
         <v>1033</v>
       </c>
-      <c r="B188" s="21"/>
-      <c r="C188" s="21"/>
-      <c r="D188" s="21"/>
-      <c r="E188" s="21"/>
-      <c r="F188" s="21"/>
-      <c r="G188" s="21"/>
-      <c r="H188" s="22"/>
+      <c r="B188" s="24"/>
+      <c r="C188" s="24"/>
+      <c r="D188" s="24"/>
+      <c r="E188" s="24"/>
+      <c r="F188" s="24"/>
+      <c r="G188" s="24"/>
+      <c r="H188" s="25"/>
     </row>
     <row r="189" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="8" t="s">
@@ -33377,16 +33402,16 @@
       </c>
     </row>
     <row r="198" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="35" t="s">
+      <c r="A198" s="29" t="s">
         <v>1088</v>
       </c>
-      <c r="B198" s="36"/>
-      <c r="C198" s="36"/>
-      <c r="D198" s="36"/>
-      <c r="E198" s="36"/>
-      <c r="F198" s="36"/>
-      <c r="G198" s="36"/>
-      <c r="H198" s="37"/>
+      <c r="B198" s="30"/>
+      <c r="C198" s="30"/>
+      <c r="D198" s="30"/>
+      <c r="E198" s="30"/>
+      <c r="F198" s="30"/>
+      <c r="G198" s="30"/>
+      <c r="H198" s="31"/>
     </row>
     <row r="199" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="3" t="s">
@@ -33571,40 +33596,40 @@
       </c>
     </row>
     <row r="206" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A206" s="20" t="s">
+      <c r="A206" s="23" t="s">
         <v>1131</v>
       </c>
-      <c r="B206" s="21"/>
-      <c r="C206" s="21"/>
-      <c r="D206" s="21"/>
-      <c r="E206" s="21"/>
-      <c r="F206" s="21"/>
-      <c r="G206" s="21"/>
-      <c r="H206" s="22"/>
+      <c r="B206" s="24"/>
+      <c r="C206" s="24"/>
+      <c r="D206" s="24"/>
+      <c r="E206" s="24"/>
+      <c r="F206" s="24"/>
+      <c r="G206" s="24"/>
+      <c r="H206" s="25"/>
     </row>
     <row r="207" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A207" s="35" t="s">
+      <c r="A207" s="29" t="s">
         <v>1132</v>
       </c>
-      <c r="B207" s="36"/>
-      <c r="C207" s="36"/>
-      <c r="D207" s="36"/>
-      <c r="E207" s="36"/>
-      <c r="F207" s="36"/>
-      <c r="G207" s="36"/>
-      <c r="H207" s="37"/>
+      <c r="B207" s="30"/>
+      <c r="C207" s="30"/>
+      <c r="D207" s="30"/>
+      <c r="E207" s="30"/>
+      <c r="F207" s="30"/>
+      <c r="G207" s="30"/>
+      <c r="H207" s="31"/>
     </row>
     <row r="208" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A208" s="35" t="s">
+      <c r="A208" s="29" t="s">
         <v>1133</v>
       </c>
-      <c r="B208" s="36"/>
-      <c r="C208" s="36"/>
-      <c r="D208" s="36"/>
-      <c r="E208" s="36"/>
-      <c r="F208" s="36"/>
-      <c r="G208" s="36"/>
-      <c r="H208" s="37"/>
+      <c r="B208" s="30"/>
+      <c r="C208" s="30"/>
+      <c r="D208" s="30"/>
+      <c r="E208" s="30"/>
+      <c r="F208" s="30"/>
+      <c r="G208" s="30"/>
+      <c r="H208" s="31"/>
     </row>
     <row r="209" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="8" t="s">
@@ -33711,28 +33736,28 @@
       </c>
     </row>
     <row r="213" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A213" s="20" t="s">
+      <c r="A213" s="23" t="s">
         <v>1158</v>
       </c>
-      <c r="B213" s="21"/>
-      <c r="C213" s="21"/>
-      <c r="D213" s="21"/>
-      <c r="E213" s="21"/>
-      <c r="F213" s="21"/>
-      <c r="G213" s="21"/>
-      <c r="H213" s="22"/>
+      <c r="B213" s="24"/>
+      <c r="C213" s="24"/>
+      <c r="D213" s="24"/>
+      <c r="E213" s="24"/>
+      <c r="F213" s="24"/>
+      <c r="G213" s="24"/>
+      <c r="H213" s="25"/>
     </row>
     <row r="214" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A214" s="20" t="s">
+      <c r="A214" s="23" t="s">
         <v>1159</v>
       </c>
-      <c r="B214" s="21"/>
-      <c r="C214" s="21"/>
-      <c r="D214" s="21"/>
-      <c r="E214" s="21"/>
-      <c r="F214" s="21"/>
-      <c r="G214" s="21"/>
-      <c r="H214" s="22"/>
+      <c r="B214" s="24"/>
+      <c r="C214" s="24"/>
+      <c r="D214" s="24"/>
+      <c r="E214" s="24"/>
+      <c r="F214" s="24"/>
+      <c r="G214" s="24"/>
+      <c r="H214" s="25"/>
     </row>
     <row r="215" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="8" t="s">
@@ -33767,22 +33792,22 @@
       <c r="B216" s="26" t="s">
         <v>1169</v>
       </c>
-      <c r="C216" s="29" t="s">
+      <c r="C216" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D216" s="29" t="s">
+      <c r="D216" s="21" t="s">
         <v>1170</v>
       </c>
-      <c r="E216" s="29" t="s">
+      <c r="E216" s="21" t="s">
         <v>1171</v>
       </c>
-      <c r="F216" s="29">
+      <c r="F216" s="21">
         <v>654</v>
       </c>
-      <c r="G216" s="29" t="s">
+      <c r="G216" s="21" t="s">
         <v>1172</v>
       </c>
-      <c r="H216" s="29" t="s">
+      <c r="H216" s="21" t="s">
         <v>1173</v>
       </c>
     </row>
@@ -33790,25 +33815,25 @@
       <c r="A217" s="15" t="s">
         <v>1167</v>
       </c>
-      <c r="B217" s="27"/>
-      <c r="C217" s="30"/>
-      <c r="D217" s="30"/>
-      <c r="E217" s="30"/>
-      <c r="F217" s="30"/>
-      <c r="G217" s="30"/>
-      <c r="H217" s="30"/>
+      <c r="B217" s="32"/>
+      <c r="C217" s="28"/>
+      <c r="D217" s="28"/>
+      <c r="E217" s="28"/>
+      <c r="F217" s="28"/>
+      <c r="G217" s="28"/>
+      <c r="H217" s="28"/>
     </row>
     <row r="218" spans="1:8" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="16" t="s">
         <v>1168</v>
       </c>
-      <c r="B218" s="28"/>
-      <c r="C218" s="31"/>
-      <c r="D218" s="31"/>
-      <c r="E218" s="31"/>
-      <c r="F218" s="31"/>
-      <c r="G218" s="31"/>
-      <c r="H218" s="31"/>
+      <c r="B218" s="27"/>
+      <c r="C218" s="22"/>
+      <c r="D218" s="22"/>
+      <c r="E218" s="22"/>
+      <c r="F218" s="22"/>
+      <c r="G218" s="22"/>
+      <c r="H218" s="22"/>
     </row>
     <row r="219" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="3" t="s">
@@ -34045,16 +34070,16 @@
       </c>
     </row>
     <row r="228" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A228" s="20" t="s">
+      <c r="A228" s="23" t="s">
         <v>1228</v>
       </c>
-      <c r="B228" s="21"/>
-      <c r="C228" s="21"/>
-      <c r="D228" s="21"/>
-      <c r="E228" s="21"/>
-      <c r="F228" s="21"/>
-      <c r="G228" s="21"/>
-      <c r="H228" s="22"/>
+      <c r="B228" s="24"/>
+      <c r="C228" s="24"/>
+      <c r="D228" s="24"/>
+      <c r="E228" s="24"/>
+      <c r="F228" s="24"/>
+      <c r="G228" s="24"/>
+      <c r="H228" s="25"/>
     </row>
     <row r="229" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="3" t="s">
@@ -34187,16 +34212,16 @@
       </c>
     </row>
     <row r="234" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="20" t="s">
+      <c r="A234" s="23" t="s">
         <v>1259</v>
       </c>
-      <c r="B234" s="21"/>
-      <c r="C234" s="21"/>
-      <c r="D234" s="21"/>
-      <c r="E234" s="21"/>
-      <c r="F234" s="21"/>
-      <c r="G234" s="21"/>
-      <c r="H234" s="22"/>
+      <c r="B234" s="24"/>
+      <c r="C234" s="24"/>
+      <c r="D234" s="24"/>
+      <c r="E234" s="24"/>
+      <c r="F234" s="24"/>
+      <c r="G234" s="24"/>
+      <c r="H234" s="25"/>
     </row>
     <row r="235" spans="1:8" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="8" t="s">
@@ -34381,16 +34406,16 @@
       </c>
     </row>
     <row r="242" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A242" s="35" t="s">
+      <c r="A242" s="29" t="s">
         <v>1302</v>
       </c>
-      <c r="B242" s="36"/>
-      <c r="C242" s="36"/>
-      <c r="D242" s="36"/>
-      <c r="E242" s="36"/>
-      <c r="F242" s="36"/>
-      <c r="G242" s="36"/>
-      <c r="H242" s="37"/>
+      <c r="B242" s="30"/>
+      <c r="C242" s="30"/>
+      <c r="D242" s="30"/>
+      <c r="E242" s="30"/>
+      <c r="F242" s="30"/>
+      <c r="G242" s="30"/>
+      <c r="H242" s="31"/>
     </row>
     <row r="243" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="3" t="s">
@@ -34529,22 +34554,22 @@
       <c r="B248" s="26" t="s">
         <v>1335</v>
       </c>
-      <c r="C248" s="29" t="s">
+      <c r="C248" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="D248" s="29" t="s">
+      <c r="D248" s="21" t="s">
         <v>1336</v>
       </c>
-      <c r="E248" s="29" t="s">
+      <c r="E248" s="21" t="s">
         <v>1337</v>
       </c>
-      <c r="F248" s="29">
+      <c r="F248" s="21">
         <v>744</v>
       </c>
-      <c r="G248" s="29" t="s">
+      <c r="G248" s="21" t="s">
         <v>1338</v>
       </c>
-      <c r="H248" s="29" t="s">
+      <c r="H248" s="21" t="s">
         <v>1339</v>
       </c>
     </row>
@@ -34552,13 +34577,13 @@
       <c r="A249" s="16" t="s">
         <v>1334</v>
       </c>
-      <c r="B249" s="28"/>
-      <c r="C249" s="31"/>
-      <c r="D249" s="31"/>
-      <c r="E249" s="31"/>
-      <c r="F249" s="31"/>
-      <c r="G249" s="31"/>
-      <c r="H249" s="31"/>
+      <c r="B249" s="27"/>
+      <c r="C249" s="22"/>
+      <c r="D249" s="22"/>
+      <c r="E249" s="22"/>
+      <c r="F249" s="22"/>
+      <c r="G249" s="22"/>
+      <c r="H249" s="22"/>
     </row>
     <row r="250" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="3" t="s">
@@ -35159,16 +35184,16 @@
       </c>
     </row>
     <row r="273" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A273" s="20" t="s">
+      <c r="A273" s="23" t="s">
         <v>1479</v>
       </c>
-      <c r="B273" s="21"/>
-      <c r="C273" s="21"/>
-      <c r="D273" s="21"/>
-      <c r="E273" s="21"/>
-      <c r="F273" s="21"/>
-      <c r="G273" s="21"/>
-      <c r="H273" s="22"/>
+      <c r="B273" s="24"/>
+      <c r="C273" s="24"/>
+      <c r="D273" s="24"/>
+      <c r="E273" s="24"/>
+      <c r="F273" s="24"/>
+      <c r="G273" s="24"/>
+      <c r="H273" s="25"/>
     </row>
     <row r="274" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" s="3" t="s">
@@ -35249,16 +35274,16 @@
       </c>
     </row>
     <row r="277" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A277" s="20" t="s">
+      <c r="A277" s="23" t="s">
         <v>1498</v>
       </c>
-      <c r="B277" s="21"/>
-      <c r="C277" s="21"/>
-      <c r="D277" s="21"/>
-      <c r="E277" s="21"/>
-      <c r="F277" s="21"/>
-      <c r="G277" s="21"/>
-      <c r="H277" s="22"/>
+      <c r="B277" s="24"/>
+      <c r="C277" s="24"/>
+      <c r="D277" s="24"/>
+      <c r="E277" s="24"/>
+      <c r="F277" s="24"/>
+      <c r="G277" s="24"/>
+      <c r="H277" s="25"/>
     </row>
     <row r="278" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A278" s="3" t="s">
@@ -35365,16 +35390,16 @@
       </c>
     </row>
     <row r="282" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A282" s="20" t="s">
+      <c r="A282" s="23" t="s">
         <v>1523</v>
       </c>
-      <c r="B282" s="21"/>
-      <c r="C282" s="21"/>
-      <c r="D282" s="21"/>
-      <c r="E282" s="21"/>
-      <c r="F282" s="21"/>
-      <c r="G282" s="21"/>
-      <c r="H282" s="22"/>
+      <c r="B282" s="24"/>
+      <c r="C282" s="24"/>
+      <c r="D282" s="24"/>
+      <c r="E282" s="24"/>
+      <c r="F282" s="24"/>
+      <c r="G282" s="24"/>
+      <c r="H282" s="25"/>
     </row>
     <row r="283" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" s="8" t="s">
@@ -35508,43 +35533,6 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="G248:G249"/>
-    <mergeCell ref="H248:H249"/>
-    <mergeCell ref="A273:H273"/>
-    <mergeCell ref="A277:H277"/>
-    <mergeCell ref="A282:H282"/>
-    <mergeCell ref="B248:B249"/>
-    <mergeCell ref="C248:C249"/>
-    <mergeCell ref="D248:D249"/>
-    <mergeCell ref="E248:E249"/>
-    <mergeCell ref="F248:F249"/>
-    <mergeCell ref="G216:G218"/>
-    <mergeCell ref="H216:H218"/>
-    <mergeCell ref="A228:H228"/>
-    <mergeCell ref="A234:H234"/>
-    <mergeCell ref="A242:H242"/>
-    <mergeCell ref="B216:B218"/>
-    <mergeCell ref="C216:C218"/>
-    <mergeCell ref="D216:D218"/>
-    <mergeCell ref="E216:E218"/>
-    <mergeCell ref="F216:F218"/>
-    <mergeCell ref="A206:H206"/>
-    <mergeCell ref="A207:H207"/>
-    <mergeCell ref="A208:H208"/>
-    <mergeCell ref="A213:H213"/>
-    <mergeCell ref="A214:H214"/>
-    <mergeCell ref="A198:H198"/>
-    <mergeCell ref="A66:H66"/>
-    <mergeCell ref="A74:H74"/>
-    <mergeCell ref="A75:H75"/>
-    <mergeCell ref="A80:H80"/>
-    <mergeCell ref="A84:H84"/>
-    <mergeCell ref="A104:H104"/>
-    <mergeCell ref="A116:H116"/>
-    <mergeCell ref="A131:H131"/>
-    <mergeCell ref="A133:H133"/>
-    <mergeCell ref="A187:H187"/>
-    <mergeCell ref="A188:H188"/>
     <mergeCell ref="A59:H59"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A4:H4"/>
@@ -35561,6 +35549,43 @@
     <mergeCell ref="A50:H50"/>
     <mergeCell ref="A51:H51"/>
     <mergeCell ref="A57:H57"/>
+    <mergeCell ref="A198:H198"/>
+    <mergeCell ref="A66:H66"/>
+    <mergeCell ref="A74:H74"/>
+    <mergeCell ref="A75:H75"/>
+    <mergeCell ref="A80:H80"/>
+    <mergeCell ref="A84:H84"/>
+    <mergeCell ref="A104:H104"/>
+    <mergeCell ref="A116:H116"/>
+    <mergeCell ref="A131:H131"/>
+    <mergeCell ref="A133:H133"/>
+    <mergeCell ref="A187:H187"/>
+    <mergeCell ref="A188:H188"/>
+    <mergeCell ref="A206:H206"/>
+    <mergeCell ref="A207:H207"/>
+    <mergeCell ref="A208:H208"/>
+    <mergeCell ref="A213:H213"/>
+    <mergeCell ref="A214:H214"/>
+    <mergeCell ref="G216:G218"/>
+    <mergeCell ref="H216:H218"/>
+    <mergeCell ref="A228:H228"/>
+    <mergeCell ref="A234:H234"/>
+    <mergeCell ref="A242:H242"/>
+    <mergeCell ref="B216:B218"/>
+    <mergeCell ref="C216:C218"/>
+    <mergeCell ref="D216:D218"/>
+    <mergeCell ref="E216:E218"/>
+    <mergeCell ref="F216:F218"/>
+    <mergeCell ref="G248:G249"/>
+    <mergeCell ref="H248:H249"/>
+    <mergeCell ref="A273:H273"/>
+    <mergeCell ref="A277:H277"/>
+    <mergeCell ref="A282:H282"/>
+    <mergeCell ref="B248:B249"/>
+    <mergeCell ref="C248:C249"/>
+    <mergeCell ref="D248:D249"/>
+    <mergeCell ref="E248:E249"/>
+    <mergeCell ref="F248:F249"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" tooltip="Islamic Republic of Afghanistan" display="https://en.wikipedia.org/wiki/Islamic_Republic_of_Afghanistan" xr:uid="{BE3E2E65-5041-4D29-B035-F231D92DCE91}"/>
@@ -37112,12 +37137,300 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946F945F-B137-468D-AB1E-1B7F1A25B3A7}">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C1" t="str">
+        <f>_xlfn.CONCAT($E$1,A1,$E$1)</f>
+        <v>"Argentina"</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1764</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1765</v>
+      </c>
+      <c r="H1" t="str">
+        <f>_xlfn.CONCAT($F$1,C1,$G$1)</f>
+        <v>listaPaises.add("Argentina");</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C20" si="0">_xlfn.CONCAT($E$1,A2,$E$1)</f>
+        <v>"Belize"</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H20" si="1">_xlfn.CONCAT($F$1,C2,$G$1)</f>
+        <v>listaPaises.add("Belize");</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1581</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>"Bolivia"</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="1"/>
+        <v>listaPaises.add("Bolivia");</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1587</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>"Brazil"</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
+        <v>listaPaises.add("Brazil");</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>264</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>"Canada"</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v>listaPaises.add("Canada");</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>"Chile"</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>listaPaises.add("Chile");</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>642</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>"China"</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v>listaPaises.add("China");</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1602</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>"Colombia"</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
+        <v>listaPaises.add("Colombia");</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1609</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>"Cuba"</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
+        <v>listaPaises.add("Cuba");</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1616</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>"Ecuador"</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="1"/>
+        <v>listaPaises.add("Ecuador");</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1759</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>"El Salvador"</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="1"/>
+        <v>listaPaises.add("El Salvador");</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1760</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>"Estados unidos"</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="1"/>
+        <v>listaPaises.add("Estados unidos");</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1761</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>"Francia"</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
+        <v>listaPaises.add("Francia");</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1635</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>"Guatemala"</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v>listaPaises.add("Guatemala");</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>"Italia"</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
+        <v>listaPaises.add("Italia");</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>709</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>"Jamaica"</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v>listaPaises.add("Jamaica");</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>716</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>"Japan"</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="1"/>
+        <v>listaPaises.add("Japan");</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1692</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>"Nigeria"</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="1"/>
+        <v>listaPaises.add("Nigeria");</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1731</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>"Sweden"</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="1"/>
+        <v>listaPaises.add("Sweden");</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1747</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>"Uruguay"</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="1"/>
+        <v>listaPaises.add("Uruguay");</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{288413C4-A3A9-4671-9BCF-AD305C12818A}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:F238"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40992,7 +41305,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{315F15C5-621E-464A-A3FF-C61431671D39}">
   <dimension ref="B2"/>
   <sheetViews>
@@ -41006,7 +41319,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:2" ht="330" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="20" t="s">
         <v>1757</v>
       </c>
     </row>
@@ -41015,7 +41328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF24ECC-A190-4B3F-8D1C-CA6472657C35}">
   <dimension ref="A2:K4"/>
   <sheetViews>

</xml_diff>